<commit_message>
finished first draft of new layout
</commit_message>
<xml_diff>
--- a/resources/SEATTLE_TEMPLATE.xlsx
+++ b/resources/SEATTLE_TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\Programming\python\WOIDS-Sound\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BDBE70-12C0-49A8-99A8-0D756BB783EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE152EF-C816-42EB-8879-A9AF677C931C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="-3945" windowWidth="16200" windowHeight="14100" xr2:uid="{6C08E104-9442-4E06-87D5-3C5A41D74CD0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34245" windowHeight="21000" activeTab="1" xr2:uid="{6C08E104-9442-4E06-87D5-3C5A41D74CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Fill in your records in their respective sheets</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>COMPONENT</t>
-  </si>
-  <si>
-    <t>DEFICIENCY</t>
   </si>
   <si>
     <t>NOTES</t>
@@ -196,10 +193,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -254,13 +248,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427F3A0C-0052-4577-8BC6-7E427F21D87D}" name="Table1" displayName="Table1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E1048576" xr:uid="{427F3A0C-0052-4577-8BC6-7E427F21D87D}"/>
-  <tableColumns count="5">
-    <tableColumn id="3" xr3:uid="{5D15C5EE-CA33-4963-853D-E90ED4A44306}" name="ID" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CA11D2E4-3A9C-4555-B4DE-64C636F6C791}" name="ROOM" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{D9E0E1D4-4A97-4C5E-912F-D028472535C7}" name="COMPONENT" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{83C073F3-6032-402D-9504-5535BB194AB9}" name="DEFICIENCY" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427F3A0C-0052-4577-8BC6-7E427F21D87D}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D1048576" xr:uid="{427F3A0C-0052-4577-8BC6-7E427F21D87D}"/>
+  <tableColumns count="4">
+    <tableColumn id="3" xr3:uid="{5D15C5EE-CA33-4963-853D-E90ED4A44306}" name="ID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{CA11D2E4-3A9C-4555-B4DE-64C636F6C791}" name="ROOM" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D9E0E1D4-4A97-4C5E-912F-D028472535C7}" name="COMPONENT" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{BAED3D3A-4E9F-4D52-B9AD-BF13F17C5185}" name="NOTES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -566,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091FE214-A36B-4558-85AA-5FA02E73BD89}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -629,11 +622,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B32A480-81EB-46C4-A8E4-C81DBDBC01D2}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,11 +634,10 @@
     <col min="1" max="1" width="7.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="37.140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="44.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -657,9 +649,6 @@
       </c>
       <c r="D1" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
top row formatting, moved date to subheader, updated spreadsheet to match new format
</commit_message>
<xml_diff>
--- a/resources/SEATTLE_TEMPLATE.xlsx
+++ b/resources/SEATTLE_TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\Programming\python\WOIDS-Sound\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE152EF-C816-42EB-8879-A9AF677C931C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD3940E-79A0-4193-8519-57616D5C5E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34245" windowHeight="21000" activeTab="1" xr2:uid="{6C08E104-9442-4E06-87D5-3C5A41D74CD0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34245" windowHeight="21000" xr2:uid="{6C08E104-9442-4E06-87D5-3C5A41D74CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Fill in your records in their respective sheets</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -52,18 +49,6 @@
     <t>DSTT NTIS INSPECTION REPORT</t>
   </si>
   <si>
-    <t>LOCATION (C##)</t>
-  </si>
-  <si>
-    <t>STATION #ROOM#</t>
-  </si>
-  <si>
-    <t>eg: C5</t>
-  </si>
-  <si>
-    <t>eg: D7</t>
-  </si>
-  <si>
     <t>eg: April-July 2021</t>
   </si>
   <si>
@@ -71,13 +56,22 @@
   </si>
   <si>
     <t>NOTES</t>
+  </si>
+  <si>
+    <t>STATION</t>
+  </si>
+  <si>
+    <t>^ please fill this in</t>
+  </si>
+  <si>
+    <t>Please fill in your records in the next sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +117,13 @@
     </font>
     <font>
       <sz val="24"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -161,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -187,13 +188,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -248,13 +255,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427F3A0C-0052-4577-8BC6-7E427F21D87D}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D1048576" xr:uid="{427F3A0C-0052-4577-8BC6-7E427F21D87D}"/>
-  <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{5D15C5EE-CA33-4963-853D-E90ED4A44306}" name="ID" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{CA11D2E4-3A9C-4555-B4DE-64C636F6C791}" name="ROOM" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{D9E0E1D4-4A97-4C5E-912F-D028472535C7}" name="COMPONENT" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{BAED3D3A-4E9F-4D52-B9AD-BF13F17C5185}" name="NOTES" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427F3A0C-0052-4577-8BC6-7E427F21D87D}" name="Table1" displayName="Table1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E1048576" xr:uid="{427F3A0C-0052-4577-8BC6-7E427F21D87D}"/>
+  <tableColumns count="5">
+    <tableColumn id="3" xr3:uid="{5D15C5EE-CA33-4963-853D-E90ED4A44306}" name="ID" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CA11D2E4-3A9C-4555-B4DE-64C636F6C791}" name="ROOM" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{FBFEEBE4-D089-48E0-8809-8A0720B08620}" name="STATION" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{D9E0E1D4-4A97-4C5E-912F-D028472535C7}" name="COMPONENT" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{BAED3D3A-4E9F-4D52-B9AD-BF13F17C5185}" name="NOTES" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -557,62 +565,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091FE214-A36B-4558-85AA-5FA02E73BD89}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.140625" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -622,33 +614,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B32A480-81EB-46C4-A8E4-C81DBDBC01D2}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" style="8" customWidth="1"/>
+    <col min="2" max="3" width="37.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>